<commit_message>
Doco change and catalog
Uploading change to documentation file.  catalog xml also shows as changed 2/23 but I am not aware of any changes to this file.
</commit_message>
<xml_diff>
--- a/Project Documentation/Ontorat-Protege Steps to Create (2022-02-20).xlsx
+++ b/Project Documentation/Ontorat-Protege Steps to Create (2022-02-20).xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samal\Documents\GitHub\OccO_Dev\Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19396D3E-B4AA-4B9E-BCAC-4AB8C45F4214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC8C11B-48D5-4389-91D2-6011E162D692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="240" windowWidth="23850" windowHeight="12480" xr2:uid="{D837B97E-5D4F-45E3-9004-7F73EC9190E1}"/>
+    <workbookView xWindow="4590" yWindow="585" windowWidth="23850" windowHeight="12480" xr2:uid="{D837B97E-5D4F-45E3-9004-7F73EC9190E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="OccO_Steps" sheetId="1" r:id="rId1"/>
+    <sheet name="OccO_Steps_Ontorat" sheetId="1" r:id="rId1"/>
+    <sheet name="Steps_Github" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="103">
   <si>
     <t xml:space="preserve">    &lt;owl:Ontology rdf:about="https://github.com/Occupation-Ontology/OccO_Dev/levelC"/&gt;</t>
   </si>
@@ -198,13 +199,169 @@
   </si>
   <si>
     <t>NOTE: Local Github for the OccO projects is backed up to drive D: Git_Dir in the (date) Github directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cannot figure out how Github is working; I do a commit from Github desktop - with the list of local files that have changed, </t>
+  </si>
+  <si>
+    <t>but the repository on github.com does not show the added files.</t>
+  </si>
+  <si>
+    <t>NO: ALL CLEARED UP - the changes had been committed but NOT PUSHED.  When pushed (after doing a pull to get remote changes) all looks in order.</t>
+  </si>
+  <si>
+    <t>Zoom conference with Dr. He:  Reviewed occoABCD.owl in OccO_Dev to note changes; additions</t>
+  </si>
+  <si>
+    <t>Problem 1: Annotations in Protégé are identified by ID (such as IAO_0000111) rather than annotation label</t>
+  </si>
+  <si>
+    <t>Fix: Add to Protégé imports the relevant ontology (see screenshot)</t>
+  </si>
+  <si>
+    <t>Prior OWL:</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0"?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;rdf:RDF xmlns="https://github.com/Occupation-Ontology/OccO_Dev/occoABCD.owl#"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xml:base="https://github.com/Occupation-Ontology/OccO_Dev/occoABCD.owl"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:obo="http://purl.obolibrary.org/obo/"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:owl="http://www.w3.org/2002/07/owl#"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:rdf="http://www.w3.org/1999/02/22-rdf-syntax-ns#"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:xml="http://www.w3.org/XML/1998/namespace"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:xsd="http://www.w3.org/2001/XMLSchema#"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:rdfs="http://www.w3.org/2000/01/rdf-schema#"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:oboInOwl="http://www.geneontology.org/formats/oboInOwl#"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:chromosome-parts="http://purl.obolibrary.org/obo/test/chromosome-parts#"&gt; &lt;&lt;&lt;&lt; DELETED!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;owl:Ontology rdf:about="https://github.com/Occupation-Ontology/OccO_Dev/occoABCD.owl"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;obo:IAO_0000115&gt;The Occupation Ontology (OccO) is an ontology in the domain of human occupations. OccO standardizes and represented all the occupations defined in the Standard Occupational Classification (SOC) developed by the following US Federal agencies:</t>
+  </si>
+  <si>
+    <t>After Protege import of IAO and saving locally:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:dc="http://purl.org/dc/elements/1.1/"  &lt;&lt; added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:foaf="http://xmlns.com/foaf/0.1/"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;&lt; added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:terms="http://purl.org/dc/terms/"      &lt;&lt; added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     xmlns:protege="http://protege.stanford.edu/plugins/owl/protege#"  &lt;&lt; added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;obo:IAO_0000115&gt;The Occupation Ontology (OccO) is an ontology in the domain of human occupations.</t>
+  </si>
+  <si>
+    <t>Can this be added to Ontorat?</t>
+  </si>
+  <si>
+    <t>Problem 2:  Where in Ontorat input does this come from:</t>
+  </si>
+  <si>
+    <t>Problem 3:  In OccO_Dev (local), the imports and Ontofox input files directories are empty!  How did that happen?</t>
+  </si>
+  <si>
+    <t>How is each of these directories used?</t>
+  </si>
+  <si>
+    <t>On Github src/ontology imports has: IAO_imorts.owl</t>
+  </si>
+  <si>
+    <t>Ontofox has: IAO_imports.txt</t>
+  </si>
+  <si>
+    <t>recap changes: added original SOC label as *** and SOC Id as ***</t>
+  </si>
+  <si>
+    <t>added description</t>
+  </si>
+  <si>
+    <t>Added O*Net 149 occupations with two-digit suffix, causing change to OccO Id from 7 to 8 digits</t>
+  </si>
+  <si>
+    <t>Plus earlier changes:  make terms lower case, and change "and" to "or"</t>
+  </si>
+  <si>
+    <t>ToDO:</t>
+  </si>
+  <si>
+    <t>Get better understanding of imports in Protégé and also Ontorat</t>
+  </si>
+  <si>
+    <t>FIRST:  Back up local github; pull from Github and back that up as well</t>
+  </si>
+  <si>
+    <t>Run ontorat locally with IAO id's and see what changes in OWL</t>
+  </si>
+  <si>
+    <t>C:\temp\OntoRat Testing\Archive</t>
+  </si>
+  <si>
+    <t>OccO_Dev_20220222_LocalBeforePull</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        &lt;owl:imports rdf:resource="http://purl.obolibrary.org/obo/iao/2020-12-09/iao.owl"/&gt;  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;&lt;&lt;&lt;&lt; ADDED</t>
+    </r>
+  </si>
+  <si>
+    <t>Run local again: occoABCD.owl</t>
+  </si>
+  <si>
+    <t>what is there?</t>
+  </si>
+  <si>
+    <t>Add import in Protégé of IAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See what is in OWL now; save this:  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +381,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,10 +414,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -270,6 +435,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>191633</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>29536</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49346621-1D5D-44DC-8466-85E550058B6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1333500"/>
+          <a:ext cx="8116433" cy="6887536"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -569,14 +783,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC979419-D6EB-469C-ABFB-95BA3B1E73AA}">
-  <dimension ref="A2:F67"/>
+  <dimension ref="A2:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="M76" sqref="M76"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="L105" sqref="L105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -839,14 +1054,263 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>44614</v>
+      </c>
+      <c r="B69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C87" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>77</v>
+      </c>
+      <c r="D92" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>92</v>
+      </c>
+      <c r="C111" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -856,4 +1320,35 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390A5523-1AF1-4D36-AC74-DB3EE3D14CDD}">
+  <dimension ref="B2:B5"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>